<commit_message>
adding the new detailed column guide to the instructions list of sheets in the template.
</commit_message>
<xml_diff>
--- a/files/soil-health-template.xlsx
+++ b/files/soil-health-template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maegensimmonds/projects/UCANR/ca-soil-health-reports-clean/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F57605-A4FE-E648-8FDA-EC472211F164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7339D71-3427-6548-9820-F108A118B84A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5720" yWindow="500" windowWidth="45480" windowHeight="22800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="200">
   <si>
     <t>year</t>
   </si>
@@ -1420,6 +1420,32 @@
   </si>
   <si>
     <t>Sodium concentration (mg/kg)</t>
+  </si>
+  <si>
+    <r>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Detailed Column Guide</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — provides definitions and example entries for each column</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1831,11 +1857,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D52516F-F4C0-4F41-9C2D-F3AC8C356E9B}">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1874,7 +1898,9 @@
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" t="s">
+        <v>199</v>
+      </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1884,265 +1910,275 @@
       <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="7"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" s="8" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9" t="s">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="9" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="7" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" s="7" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="7"/>
-    </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" s="4" t="s">
         <v>129</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2779,7 +2815,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>